<commit_message>
Bussiness Core package devide and 3 unused mappers deleted
Signed-off-by: Chatura Galagama <chaturangalagama@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/core_service_dependancies.xlsx
+++ b/doc/core_service_dependancies.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" tabRatio="290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="66">
   <si>
     <t>label</t>
   </si>
@@ -369,14 +368,69 @@
     <t>patient [exists(followup.getPatientId())]</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>clinic_microservice</t>
+  </si>
+  <si>
+    <t>patient_microservice</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>patient_vist</t>
+  </si>
+  <si>
+    <t>clinic_microservice (only for now)</t>
+  </si>
+  <si>
+    <t>clinic_microservice(visit)</t>
+  </si>
+  <si>
+    <t>clinic_microservice(payment)</t>
+  </si>
+  <si>
+    <t>API CALL TO PATIENT - findPatientById</t>
+  </si>
+  <si>
+    <t>patient [exists(PatientId())]</t>
+  </si>
+  <si>
+    <r>
+      <t>running_number_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>service [generatePatientNumber()]</t>
+    </r>
+  </si>
+  <si>
+    <t>API CALL TO CLINIC - running_number_service [generatePatientNumber()]</t>
+  </si>
+  <si>
+    <t>patient_microservice(visit)</t>
+  </si>
+  <si>
+    <t>API CALL TO CLINIC - findOne(doctorId)</t>
+  </si>
+  <si>
+    <t>API CALL TO CLINIC - findOne(clinicId)</t>
+  </si>
+  <si>
+    <t>API CALL TO CLINIC - running_number_service [queueNextNumber()]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +528,61 @@
     <font>
       <sz val="11"/>
       <color rgb="FFD58987"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -499,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -513,6 +622,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,206 +938,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="C18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="F22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="F23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F24" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="F25" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1037,8 +1281,14 @@
       <c r="E27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1051,8 +1301,14 @@
       <c r="D28" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1062,8 +1318,14 @@
       <c r="C29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1079,8 +1341,14 @@
       <c r="E30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1098,6 +1366,26 @@
       </c>
       <c r="F31" t="s">
         <v>34</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1108,24 +1396,439 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>